<commit_message>
chore: update last_date.txt to reflect new deadline
</commit_message>
<xml_diff>
--- a/student_data/student_data.xlsx
+++ b/student_data/student_data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -545,19 +545,19 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>5/53</t>
+          <t>6/52</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update last_date.txt to reflect new deadline
</commit_message>
<xml_diff>
--- a/student_data/student_data.xlsx
+++ b/student_data/student_data.xlsx
@@ -545,8 +545,10 @@
           <t>Vernwin Kwan</t>
         </is>
       </c>
-      <c r="D2" s="2" t="n">
-        <v>41872</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2014/08/21</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -587,19 +589,19 @@
         </is>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/4</t>
         </is>
       </c>
     </row>
@@ -619,8 +621,10 @@
           <t>Yap Hee En</t>
         </is>
       </c>
-      <c r="D3" s="2" t="n">
-        <v>41220</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2012/11/07</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -661,19 +665,19 @@
         </is>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/4</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Improved GUI/normal funtion is done. left with improve some minor changes
</commit_message>
<xml_diff>
--- a/student_data/student_data.xlsx
+++ b/student_data/student_data.xlsx
@@ -545,10 +545,8 @@
           <t>Vernwin Kwan</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2014/08/21</t>
-        </is>
+      <c r="D2" s="2" t="n">
+        <v>41872</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -601,7 +599,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>1/4</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -621,10 +619,8 @@
           <t>Yap Hee En</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2012/11/07</t>
-        </is>
+      <c r="D3" s="2" t="n">
+        <v>41220</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -677,7 +673,7 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>1/4</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -739,19 +735,19 @@
         </is>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -813,19 +809,19 @@
         </is>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -887,19 +883,19 @@
         </is>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -961,19 +957,19 @@
         </is>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -1035,19 +1031,19 @@
         </is>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -1109,19 +1105,19 @@
         </is>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -1183,19 +1179,19 @@
         </is>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -1257,19 +1253,19 @@
         </is>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -1331,19 +1327,19 @@
         </is>
       </c>
       <c r="O12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -1405,19 +1401,19 @@
         </is>
       </c>
       <c r="O13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -1471,19 +1467,19 @@
         </is>
       </c>
       <c r="O14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -1545,19 +1541,19 @@
         </is>
       </c>
       <c r="O15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -1619,19 +1615,19 @@
         </is>
       </c>
       <c r="O16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -1693,19 +1689,19 @@
         </is>
       </c>
       <c r="O17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -1749,19 +1745,19 @@
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -1819,19 +1815,19 @@
         </is>
       </c>
       <c r="O19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -1885,19 +1881,19 @@
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -1951,19 +1947,19 @@
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -2025,19 +2021,19 @@
         </is>
       </c>
       <c r="O22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -2095,19 +2091,19 @@
         </is>
       </c>
       <c r="O23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -2169,19 +2165,19 @@
         </is>
       </c>
       <c r="O24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -2244,19 +2240,19 @@
         </is>
       </c>
       <c r="O25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -2318,19 +2314,19 @@
         </is>
       </c>
       <c r="O26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -2392,19 +2388,19 @@
         </is>
       </c>
       <c r="O27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -2466,19 +2462,19 @@
         </is>
       </c>
       <c r="O28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -2540,19 +2536,19 @@
         </is>
       </c>
       <c r="O29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -2614,19 +2610,19 @@
         </is>
       </c>
       <c r="O30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -2670,19 +2666,19 @@
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -2740,19 +2736,19 @@
         </is>
       </c>
       <c r="O32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R32" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -2800,19 +2796,19 @@
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -2866,19 +2862,19 @@
         </is>
       </c>
       <c r="O34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R34" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>
@@ -10655,8 +10651,10 @@
           <t>Joel Leong Yue Er</t>
         </is>
       </c>
-      <c r="D145" s="2" t="n">
-        <v>42309</v>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>2015/11/01</t>
+        </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -10685,19 +10683,19 @@
         </is>
       </c>
       <c r="O145" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P145" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q145" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R145" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added browse file function
</commit_message>
<xml_diff>
--- a/student_data/student_data.xlsx
+++ b/student_data/student_data.xlsx
@@ -545,8 +545,10 @@
           <t>Vernwin Kwan</t>
         </is>
       </c>
-      <c r="D2" s="2" t="n">
-        <v>41872</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2014/08/21</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -587,19 +589,19 @@
         </is>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add attendance system log for August 16, 2025
- Logged sign-in details including student ID, name, and time
- Handled unknown student ID error
- Printed detailed attendance records and final data before application shutdown
</commit_message>
<xml_diff>
--- a/student_data/student_data.xlsx
+++ b/student_data/student_data.xlsx
@@ -621,8 +621,10 @@
           <t>Yap Hee En</t>
         </is>
       </c>
-      <c r="D3" s="2" t="n">
-        <v>41220</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2012/11/07</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -663,19 +665,19 @@
         </is>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/52</t>
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1/5</t>
         </is>
       </c>
     </row>

</xml_diff>